<commit_message>
Updated survey result spreadsheet
</commit_message>
<xml_diff>
--- a/PA Survey Results.xlsx
+++ b/PA Survey Results.xlsx
@@ -13,8 +13,186 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Olson</author>
+  </authors>
+  <commentList>
+    <comment ref="AR3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Olson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Still need a way to communicate with FW so PA can kick-off a FW project backup or restore. Then PA can include FW data sources in its backup file.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Olson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Not high enough priority to implement.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AR7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Olson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Exporting charts in HTML is so good now, having an RTF option is not necessary.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Olson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Possibly, but not high enough priority to implement in light of other needs.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Olson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Possibly, but not high enough priority to implement in light of other needs.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Olson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+I have not had much call for this.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B12" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Olson:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+I have not had much call for this.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="54">
   <si>
     <t>Don Cheney</t>
   </si>
@@ -170,13 +348,19 @@
   </si>
   <si>
     <t>Heidi Rosendall</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>almost</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -190,6 +374,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -227,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment textRotation="180"/>
@@ -248,80 +445,18 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="180"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" textRotation="180"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
 </styleSheet>
 </file>
 
@@ -330,10 +465,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="282828"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="EFEED3"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -610,10 +745,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AQ14"/>
+  <dimension ref="A1:AR14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AC6" sqref="AC6"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -628,9 +763,10 @@
     <col min="39" max="40" width="3.28515625" customWidth="1"/>
     <col min="41" max="41" width="3.28515625" bestFit="1" customWidth="1"/>
     <col min="42" max="43" width="5.85546875" customWidth="1"/>
+    <col min="44" max="44" width="9.140625" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" s="1" customFormat="1" ht="170.25" customHeight="1">
+    <row r="1" spans="1:44" s="1" customFormat="1" ht="170.25" customHeight="1">
       <c r="A1" s="3"/>
       <c r="C1" s="7" t="s">
         <v>0</v>
@@ -755,8 +891,9 @@
       <c r="AQ1" s="9" t="s">
         <v>37</v>
       </c>
+      <c r="AR1" s="11"/>
     </row>
-    <row r="2" spans="1:43">
+    <row r="2" spans="1:44">
       <c r="A2">
         <v>1</v>
       </c>
@@ -888,8 +1025,11 @@
         <f>RANK(AP2,AP2:AP12)</f>
         <v>1</v>
       </c>
+      <c r="AR2" s="10" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="3" spans="1:43">
+    <row r="3" spans="1:44">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1020,8 +1160,11 @@
       <c r="AQ3" s="6">
         <v>5</v>
       </c>
+      <c r="AR3" s="10" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="4" spans="1:43">
+    <row r="4" spans="1:44">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1153,7 +1296,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:43">
+    <row r="5" spans="1:44">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1285,7 +1428,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:43">
+    <row r="6" spans="1:44">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1417,7 +1560,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:43">
+    <row r="7" spans="1:44">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1548,8 +1691,11 @@
       <c r="AQ7" s="6">
         <v>3</v>
       </c>
+      <c r="AR7" s="10" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="8" spans="1:43">
+    <row r="8" spans="1:44">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1681,7 +1827,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:43">
+    <row r="9" spans="1:44">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1813,7 +1959,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:43">
+    <row r="10" spans="1:44">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1945,7 +2091,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:43">
+    <row r="11" spans="1:44">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2076,8 +2222,11 @@
       <c r="AQ11" s="6">
         <v>6</v>
       </c>
+      <c r="AR11" s="10" t="s">
+        <v>52</v>
+      </c>
     </row>
-    <row r="12" spans="1:43">
+    <row r="12" spans="1:44">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2209,10 +2358,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:43">
+    <row r="13" spans="1:44">
       <c r="AQ13" s="5"/>
     </row>
-    <row r="14" spans="1:43">
+    <row r="14" spans="1:44">
       <c r="C14" s="5">
         <v>1</v>
       </c>
@@ -2373,5 +2522,6 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>